<commit_message>
Let the User to Define Place Of Supply for Each Entry in Purchase/Sales
</commit_message>
<xml_diff>
--- a/E2TGST/Resources/SalesEntries.xlsx
+++ b/E2TGST/Resources/SalesEntries.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\GST-Tally-Helper\E2TGST\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Dineshkumar\Projects\Excel-to-Tally-for-GST\E2TGST\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1F2B2DE2-17F4-4D47-9DAE-E3FE1EB35E3C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{D8A0F778-E9CD-48E6-B356-08504E8D0EF9}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Sales Entries" sheetId="1" r:id="rId1"/>
     <sheet name="List" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>GSTIN</t>
   </si>
@@ -59,12 +58,15 @@
   </si>
   <si>
     <t>GST Rates</t>
+  </si>
+  <si>
+    <t>Place of Supply</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -128,7 +130,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <protection locked="0" hidden="0"/>
@@ -190,19 +196,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6641C363-777C-4291-A848-DD31838554BF}" name="Table1" displayName="Table1" ref="A1:J99" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
-  <autoFilter ref="A1:J99" xr:uid="{ACCD32B7-FD0B-4A65-9D67-7610869FA679}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{E0F9E751-B0BD-4FEB-974E-46F0957EA1EB}" name="GSTIN" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{E6F56B07-F31F-4E6B-B0B8-B1642FDFA0E0}" name="Invoice Date" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{F2D5E89F-EBC5-4F91-BC6A-503094717339}" name="Invoice Number" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{1BEF6519-2DB3-480C-8C69-2823C29BA599}" name="Invoice Value" dataDxfId="6"/>
-    <tableColumn id="5" xr3:uid="{B8DBA688-939B-4677-AA04-BB67BC7CF218}" name="Rate" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{4B322682-32D3-4993-B481-066B72CFB345}" name="Taxable Value" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{7F834F94-0BB3-45D3-A2CD-C296C3D64C6F}" name="IGST" dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{F3EB9593-863C-490B-A566-87D8B8597B20}" name="CGST" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{5112CCD4-8D3E-4422-BE83-2FE2C8EF79DB}" name="SGST" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{83A779B3-5913-4825-90A0-310F2A4E4099}" name="CESS" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K99" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A1:K99"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="GSTIN" dataDxfId="10"/>
+    <tableColumn id="2" name="Invoice Date" dataDxfId="9"/>
+    <tableColumn id="3" name="Invoice Number" dataDxfId="8"/>
+    <tableColumn id="4" name="Invoice Value" dataDxfId="7"/>
+    <tableColumn id="5" name="Rate" dataDxfId="6"/>
+    <tableColumn id="6" name="Taxable Value" dataDxfId="5"/>
+    <tableColumn id="7" name="IGST" dataDxfId="4"/>
+    <tableColumn id="8" name="CGST" dataDxfId="3"/>
+    <tableColumn id="9" name="SGST" dataDxfId="2"/>
+    <tableColumn id="10" name="CESS" dataDxfId="1"/>
+    <tableColumn id="11" name="Place of Supply" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -504,9 +511,9 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8AC1771-6EC9-4AFC-9ACE-4FF5B99E830E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="SalesEntries"/>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:K99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -523,10 +530,11 @@
     <col min="7" max="8" width="9.140625" style="5" customWidth="1"/>
     <col min="9" max="9" width="7.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="5" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1" hidden="1"/>
+    <col min="11" max="11" width="19" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -557,9 +565,306 @@
       <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="5"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="5"/>
+    </row>
+    <row r="18" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K18" s="5"/>
+    </row>
+    <row r="19" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K19" s="5"/>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K20" s="5"/>
+    </row>
+    <row r="21" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="5"/>
+    </row>
+    <row r="22" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="5"/>
+    </row>
+    <row r="23" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="5"/>
+    </row>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="5"/>
+    </row>
+    <row r="25" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K25" s="5"/>
+    </row>
+    <row r="26" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="5"/>
+    </row>
+    <row r="27" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="5"/>
+    </row>
+    <row r="28" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="5"/>
+    </row>
+    <row r="29" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K29" s="5"/>
+    </row>
+    <row r="30" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K30" s="5"/>
+    </row>
+    <row r="31" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K31" s="5"/>
+    </row>
+    <row r="32" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K32" s="5"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="5"/>
+    </row>
+    <row r="34" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K34" s="5"/>
+    </row>
+    <row r="35" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K35" s="5"/>
+    </row>
+    <row r="36" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K36" s="5"/>
+    </row>
+    <row r="37" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K37" s="5"/>
+    </row>
+    <row r="38" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K38" s="5"/>
+    </row>
+    <row r="39" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K39" s="5"/>
+    </row>
+    <row r="40" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K40" s="5"/>
+    </row>
+    <row r="41" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K41" s="5"/>
+    </row>
+    <row r="42" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K42" s="5"/>
+    </row>
+    <row r="43" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K43" s="5"/>
+    </row>
+    <row r="44" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K44" s="5"/>
+    </row>
+    <row r="45" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K45" s="5"/>
+    </row>
+    <row r="46" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K46" s="5"/>
+    </row>
+    <row r="47" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K47" s="5"/>
+    </row>
+    <row r="48" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K48" s="5"/>
+    </row>
+    <row r="49" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K49" s="5"/>
+    </row>
+    <row r="50" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K50" s="5"/>
+    </row>
+    <row r="51" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K51" s="5"/>
+    </row>
+    <row r="52" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K52" s="5"/>
+    </row>
+    <row r="53" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K53" s="5"/>
+    </row>
+    <row r="54" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K54" s="5"/>
+    </row>
+    <row r="55" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K55" s="5"/>
+    </row>
+    <row r="56" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K56" s="5"/>
+    </row>
+    <row r="57" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K57" s="5"/>
+    </row>
+    <row r="58" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K58" s="5"/>
+    </row>
+    <row r="59" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K59" s="5"/>
+    </row>
+    <row r="60" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K60" s="5"/>
+    </row>
+    <row r="61" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K61" s="5"/>
+    </row>
+    <row r="62" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="5"/>
+    </row>
+    <row r="63" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K63" s="5"/>
+    </row>
+    <row r="64" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K64" s="5"/>
+    </row>
+    <row r="65" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="5"/>
+    </row>
+    <row r="66" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="5"/>
+    </row>
+    <row r="67" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K67" s="5"/>
+    </row>
+    <row r="68" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="5"/>
+    </row>
+    <row r="69" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K69" s="5"/>
+    </row>
+    <row r="70" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K70" s="5"/>
+    </row>
+    <row r="71" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K71" s="5"/>
+    </row>
+    <row r="72" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K72" s="5"/>
+    </row>
+    <row r="73" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K73" s="5"/>
+    </row>
+    <row r="74" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K74" s="5"/>
+    </row>
+    <row r="75" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K75" s="5"/>
+    </row>
+    <row r="76" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K76" s="5"/>
+    </row>
+    <row r="77" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K77" s="5"/>
+    </row>
+    <row r="78" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K78" s="5"/>
+    </row>
+    <row r="79" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K79" s="5"/>
+    </row>
+    <row r="80" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K80" s="5"/>
+    </row>
+    <row r="81" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K81" s="5"/>
+    </row>
+    <row r="82" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K82" s="5"/>
+    </row>
+    <row r="83" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K83" s="5"/>
+    </row>
+    <row r="84" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K84" s="5"/>
+    </row>
+    <row r="85" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K85" s="5"/>
+    </row>
+    <row r="86" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K86" s="5"/>
+    </row>
+    <row r="87" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K87" s="5"/>
+    </row>
+    <row r="88" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K88" s="5"/>
+    </row>
+    <row r="89" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K89" s="5"/>
+    </row>
+    <row r="90" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K90" s="5"/>
+    </row>
+    <row r="91" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K91" s="5"/>
+    </row>
+    <row r="92" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K92" s="5"/>
+    </row>
+    <row r="93" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K93" s="5"/>
+    </row>
+    <row r="94" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K94" s="5"/>
+    </row>
+    <row r="95" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K95" s="5"/>
+    </row>
+    <row r="96" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K96" s="5"/>
+    </row>
+    <row r="97" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K97" s="5"/>
+    </row>
+    <row r="98" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K98" s="5"/>
+    </row>
+    <row r="99" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K99" s="5"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="5xxus25WFf6/e63I4n6PWjXhMZyYGoyZ0lu3+X9aF2zzFw2piRnj9Jc+pir0b6AZHvO97RVUnVO00VCGEm/VCg==" saltValue="8LlutjVk7855AIOQ4RC6Ow==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="lY4eHfCfpukvqXiN7RJe8UjapnzHXlsn2n1IMi+K4njC4lD/4mW52qfbsRsLCDTBVk1DleyP2cgX7EonjoM2tw==" saltValue="YJsY50iHAFUMd1tQfHFQ6g==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatColumns="0" insertRows="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -568,7 +873,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43D42C5B-6F11-4C32-90AA-46403DD79AE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="List"/>
   <dimension ref="A1:A6"/>
   <sheetViews>

</xml_diff>